<commit_message>
Criação do processo de Automação Fakturama
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://certsysti-my.sharepoint.com/personal/samuel_perroni_certsys_com_br/Documents/Documentos/UiPath/AutomaçãoFakturama_Perf/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEEBA2C4-0B5C-4583-BC75-52F21486253B}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6125C588-8980-4743-B850-57B5BBB50B44}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Fakturama_ProductsPath</t>
+  </si>
+  <si>
+    <t>Diretório padrão onde estão adicionados as imagens para uso no Fakturama</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2791,7 +2794,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2844,6 +2847,12 @@
       </c>
       <c r="B2" t="s">
         <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>